<commit_message>
Columns that should be discarded
</commit_message>
<xml_diff>
--- a/LCDataDictionary.xlsx
+++ b/LCDataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bojri\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire\Desktop\DSBD\Project 2\DSBD-LendingClub-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAD782D-1812-4A27-935D-DE167847168B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A41390C-DB21-4848-8734-577E333DD389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -1133,7 +1133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1316,6 +1316,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1554,7 +1560,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1576,10 +1582,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="92">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1981,19 +1998,19 @@
   <dimension ref="A1:K154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A145" sqref="A145:B145"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="196.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.77734375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="90.6328125" customWidth="1"/>
+    <col min="3" max="3" width="118.81640625" style="6" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>93</v>
       </c>
@@ -2001,7 +2018,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>213</v>
       </c>
@@ -2010,7 +2027,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>217</v>
       </c>
@@ -2019,7 +2036,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -2028,7 +2045,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>207</v>
       </c>
@@ -2037,7 +2054,7 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -2046,16 +2063,15 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>174</v>
       </c>
@@ -2064,7 +2080,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>107</v>
       </c>
@@ -2073,7 +2089,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>218</v>
       </c>
@@ -2082,7 +2098,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>219</v>
       </c>
@@ -2091,7 +2107,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>98</v>
       </c>
@@ -2100,16 +2116,15 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>99</v>
       </c>
@@ -2118,34 +2133,33 @@
       </c>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="16"/>
-    </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>220</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="16"/>
-    </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="C16" s="15"/>
+    </row>
+    <row r="17" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:3" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -2154,16 +2168,15 @@
       </c>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -2172,7 +2185,7 @@
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -2181,16 +2194,15 @@
       </c>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
@@ -2199,7 +2211,7 @@
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2208,25 +2220,23 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+    </row>
+    <row r="26" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>8</v>
       </c>
@@ -2235,7 +2245,7 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
@@ -2244,25 +2254,25 @@
       </c>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="16"/>
-    </row>
-    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="18"/>
+    </row>
+    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>199</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C30" s="16"/>
-    </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="15"/>
+    </row>
+    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
@@ -2271,7 +2281,7 @@
       </c>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>209</v>
       </c>
@@ -2280,7 +2290,7 @@
       </c>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>211</v>
       </c>
@@ -2289,7 +2299,7 @@
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>26</v>
       </c>
@@ -2298,7 +2308,7 @@
       </c>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2307,7 +2317,7 @@
       </c>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
@@ -2316,7 +2326,7 @@
       </c>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>13</v>
       </c>
@@ -2327,16 +2337,15 @@
       <c r="I37" s="10"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>46</v>
       </c>
@@ -2345,7 +2354,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>47</v>
       </c>
@@ -2354,25 +2363,25 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:11" s="20" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+      <c r="D41" s="19"/>
+    </row>
+    <row r="42" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="19"/>
+    </row>
+    <row r="43" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
@@ -2381,7 +2390,7 @@
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -2390,7 +2399,7 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>205</v>
       </c>
@@ -2399,19 +2408,19 @@
       </c>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D46" s="4"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D46" s="19"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>221</v>
       </c>
@@ -2423,7 +2432,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>117</v>
       </c>
@@ -2435,7 +2444,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>118</v>
       </c>
@@ -2444,7 +2453,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>104</v>
       </c>
@@ -2453,7 +2462,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>222</v>
       </c>
@@ -2462,7 +2471,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>27</v>
       </c>
@@ -2471,7 +2480,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
         <v>101</v>
       </c>
@@ -2480,7 +2489,7 @@
       </c>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>28</v>
       </c>
@@ -2489,7 +2498,7 @@
       </c>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>195</v>
       </c>
@@ -2498,7 +2507,7 @@
       </c>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>223</v>
       </c>
@@ -2507,7 +2516,7 @@
       </c>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="8" t="s">
         <v>224</v>
       </c>
@@ -2516,7 +2525,7 @@
       </c>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>226</v>
       </c>
@@ -2525,7 +2534,7 @@
       </c>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>227</v>
       </c>
@@ -2534,16 +2543,16 @@
       </c>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
+    <row r="60" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D60" s="4"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D60" s="19"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>97</v>
       </c>
@@ -2552,7 +2561,7 @@
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>109</v>
       </c>
@@ -2560,7 +2569,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>116</v>
       </c>
@@ -2568,7 +2577,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
         <v>110</v>
       </c>
@@ -2576,7 +2585,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="9" t="s">
         <v>108</v>
       </c>
@@ -2584,7 +2593,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>115</v>
       </c>
@@ -2592,7 +2601,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
         <v>120</v>
       </c>
@@ -2600,7 +2609,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
         <v>95</v>
       </c>
@@ -2608,7 +2617,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
         <v>119</v>
       </c>
@@ -2616,7 +2625,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
         <v>102</v>
       </c>
@@ -2624,23 +2633,23 @@
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="9" t="s">
+    <row r="71" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="9" t="s">
+    <row r="72" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="16" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
         <v>112</v>
       </c>
@@ -2650,7 +2659,7 @@
       <c r="C73"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
         <v>103</v>
       </c>
@@ -2658,7 +2667,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>29</v>
       </c>
@@ -2666,7 +2675,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
         <v>188</v>
       </c>
@@ -2674,7 +2683,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
         <v>191</v>
       </c>
@@ -2682,7 +2691,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
         <v>193</v>
       </c>
@@ -2690,7 +2699,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="s">
         <v>257</v>
       </c>
@@ -2698,7 +2707,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
         <v>201</v>
       </c>
@@ -2706,7 +2715,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="9" t="s">
         <v>203</v>
       </c>
@@ -2714,23 +2723,23 @@
         <v>204</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
+    <row r="82" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
+    <row r="83" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="9" t="s">
         <v>111</v>
       </c>
@@ -2738,7 +2747,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="9" t="s">
         <v>228</v>
       </c>
@@ -2746,15 +2755,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A86" s="3" t="s">
+    <row r="86" spans="1:2" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A86" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="17" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>30</v>
       </c>
@@ -2762,7 +2771,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="9" t="s">
         <v>96</v>
       </c>
@@ -2770,7 +2779,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>18</v>
       </c>
@@ -2778,15 +2787,15 @@
         <v>164</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
+    <row r="90" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B90" s="17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="7" t="s">
         <v>162</v>
       </c>
@@ -2794,7 +2803,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>31</v>
       </c>
@@ -2802,7 +2811,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>32</v>
       </c>
@@ -2810,7 +2819,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>9</v>
       </c>
@@ -2818,7 +2827,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="9" t="s">
         <v>100</v>
       </c>
@@ -2826,7 +2835,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>5</v>
       </c>
@@ -2834,15 +2843,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="3" t="s">
+    <row r="97" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="17" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="9" t="s">
         <v>121</v>
       </c>
@@ -2850,7 +2859,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="9" t="s">
         <v>106</v>
       </c>
@@ -2858,7 +2867,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="9" t="s">
         <v>105</v>
       </c>
@@ -2866,7 +2875,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>33</v>
       </c>
@@ -2874,7 +2883,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="9" t="s">
         <v>229</v>
       </c>
@@ -2882,7 +2891,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="s">
         <v>197</v>
       </c>
@@ -2890,7 +2899,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="9" t="s">
         <v>230</v>
       </c>
@@ -2898,7 +2907,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="9" t="s">
         <v>215</v>
       </c>
@@ -2906,7 +2915,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="9" t="s">
         <v>94</v>
       </c>
@@ -2914,47 +2923,47 @@
         <v>150</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="3" t="s">
+    <row r="107" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="3" t="s">
+    <row r="108" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="3" t="s">
+    <row r="109" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B109" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="3" t="s">
+    <row r="110" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B110" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="3" t="s">
+    <row r="111" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B111" s="17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="9" t="s">
         <v>156</v>
       </c>
@@ -2962,15 +2971,15 @@
         <v>151</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="3" t="s">
+    <row r="113" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B113" s="17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="7" t="s">
         <v>216</v>
       </c>
@@ -2978,311 +2987,311 @@
         <v>159</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="7" t="s">
+    <row r="115" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="B115" s="7" t="s">
+      <c r="B115" s="16" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="15" t="s">
+    <row r="116" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="B116" s="15" t="s">
+      <c r="B116" s="23" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="15" t="s">
+    <row r="117" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="B117" s="15" t="s">
+      <c r="B117" s="23" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="15" t="s">
+    <row r="118" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="B118" s="15" t="s">
+      <c r="B118" s="23" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="15" t="s">
+    <row r="119" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="B119" s="15" t="s">
+      <c r="B119" s="23" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="15" t="s">
+    <row r="120" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="B120" s="15" t="s">
+      <c r="B120" s="23" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="15" t="s">
+    <row r="121" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="23" t="s">
         <v>240</v>
       </c>
-      <c r="B121" s="15" t="s">
+      <c r="B121" s="23" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="15" t="s">
+    <row r="122" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="23" t="s">
         <v>242</v>
       </c>
-      <c r="B122" s="15" t="s">
+      <c r="B122" s="23" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="15" t="s">
+    <row r="123" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="23" t="s">
         <v>244</v>
       </c>
-      <c r="B123" s="15" t="s">
+      <c r="B123" s="23" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="15" t="s">
+    <row r="124" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="B124" s="15" t="s">
+      <c r="B124" s="23" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="15" t="s">
+    <row r="125" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="B125" s="15" t="s">
+      <c r="B125" s="23" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="15" t="s">
+    <row r="126" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="B126" s="15" t="s">
+      <c r="B126" s="23" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="15" t="s">
+    <row r="127" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="B127" s="15" t="s">
+      <c r="B127" s="23" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="15" t="s">
+    <row r="128" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="23" t="s">
         <v>253</v>
       </c>
-      <c r="B128" s="15" t="s">
+      <c r="B128" s="23" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="15" t="s">
+    <row r="129" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A129" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="B129" s="15" t="s">
+      <c r="B129" s="23" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="9" t="s">
+    <row r="130" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="B130" s="9" t="s">
+      <c r="B130" s="22" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="9" t="s">
+    <row r="131" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="B131" s="9" t="s">
+      <c r="B131" s="22" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="9" t="s">
+    <row r="132" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="B132" s="9" t="s">
+      <c r="B132" s="22" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="9" t="s">
+    <row r="133" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A133" s="22" t="s">
         <v>272</v>
       </c>
-      <c r="B133" s="9" t="s">
+      <c r="B133" s="22" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="9" t="s">
+    <row r="134" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A134" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="B134" s="9" t="s">
+      <c r="B134" s="22" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" s="9" t="s">
+    <row r="135" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A135" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="B135" s="9" t="s">
+      <c r="B135" s="22" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="9" t="s">
+    <row r="136" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A136" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="B136" s="9" t="s">
+      <c r="B136" s="22" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="9" t="s">
+    <row r="137" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A137" s="22" t="s">
         <v>276</v>
       </c>
-      <c r="B137" s="9" t="s">
+      <c r="B137" s="22" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="9" t="s">
+    <row r="138" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A138" s="22" t="s">
         <v>277</v>
       </c>
-      <c r="B138" s="9" t="s">
+      <c r="B138" s="22" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" s="9" t="s">
+    <row r="139" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A139" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="B139" s="9" t="s">
+      <c r="B139" s="22" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="9" t="s">
+    <row r="140" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A140" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="B140" s="9" t="s">
+      <c r="B140" s="22" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" s="9" t="s">
+    <row r="141" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="B141" s="9" t="s">
+      <c r="B141" s="22" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" s="9" t="s">
+    <row r="142" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A142" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="B142" s="9" t="s">
+      <c r="B142" s="22" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" s="9" t="s">
+    <row r="143" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A143" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="B143" s="9" t="s">
+      <c r="B143" s="22" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" s="9" t="s">
+    <row r="144" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A144" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="B144" s="9" t="s">
+      <c r="B144" s="22" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" s="9" t="s">
+    <row r="145" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A145" s="22" t="s">
         <v>284</v>
       </c>
-      <c r="B145" s="9" t="s">
+      <c r="B145" s="22" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="9" t="s">
+    <row r="146" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A146" s="22" t="s">
         <v>267</v>
       </c>
-      <c r="B146" s="9" t="s">
+      <c r="B146" s="22" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="9" t="s">
+    <row r="147" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A147" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="B147" s="9" t="s">
+      <c r="B147" s="22" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A148" s="9" t="s">
+    <row r="148" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A148" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="B148" s="9" t="s">
+      <c r="B148" s="22" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A149" s="9" t="s">
+    <row r="149" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A149" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="B149" s="9" t="s">
+      <c r="B149" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A150" s="9" t="s">
+    <row r="150" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="B150" s="9" t="s">
+      <c r="B150" s="22" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A151" s="9" t="s">
+    <row r="151" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A151" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="B151" s="9" t="s">
+      <c r="B151" s="22" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" s="9" t="s">
+    <row r="152" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="B152" s="9" t="s">
+      <c r="B152" s="22" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B154" s="13" t="s">
         <v>155</v>
       </c>

</xml_diff>